<commit_message>
MAJ 26/04/2024 - avancement script critères liste rouge régionale
</commit_message>
<xml_diff>
--- a/raw_data/selection_taxon_lrr.xlsx
+++ b/raw_data/selection_taxon_lrr.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lea.bouchet\Documents\Artif\Artif\liste_rouge_regionale\raw_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F3354DF-0E15-4785-B2DD-332B6A67CD12}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D0E253E-1F3E-4CC0-9C16-96CDB16C75B3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{25E8E10F-A282-45EE-82C4-3240378E5878}"/>
   </bookViews>
@@ -724,8 +724,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68C65F63-35D5-4CD1-B443-72BB0835CA8F}">
   <dimension ref="A1:E50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1344,6 +1344,9 @@
       <c r="C40" s="1" t="s">
         <v>66</v>
       </c>
+      <c r="D40" s="1">
+        <v>10</v>
+      </c>
       <c r="E40" s="1" t="s">
         <v>105</v>
       </c>

</xml_diff>

<commit_message>
MAJ - Travail critères LRR
</commit_message>
<xml_diff>
--- a/raw_data/selection_taxon_lrr.xlsx
+++ b/raw_data/selection_taxon_lrr.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lea.bouchet\Documents\Artif\Artif\liste_rouge_regionale\raw_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DA96B0C-17A2-45B8-B29B-05FFE26136EB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C13409B-11AD-47D8-A607-E49F2A40D609}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{25E8E10F-A282-45EE-82C4-3240378E5878}"/>
   </bookViews>
@@ -724,7 +724,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68C65F63-35D5-4CD1-B443-72BB0835CA8F}">
   <dimension ref="A1:E50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
@@ -1127,7 +1127,7 @@
         <v>85</v>
       </c>
       <c r="D27" s="1">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>104</v>

</xml_diff>

<commit_message>
Mise à jour 25/06
</commit_message>
<xml_diff>
--- a/raw_data/selection_taxon_lrr.xlsx
+++ b/raw_data/selection_taxon_lrr.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20411"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lea.bouchet\Documents\Artif\Artif\liste_rouge_regionale\raw_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D31E1FFA-72A2-49EB-871A-EF65691488C5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E392F9D-2B42-4413-B592-1C54ED56D954}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{25E8E10F-A282-45EE-82C4-3240378E5878}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil1!$A$1:$E$50</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil1!$A$1:$F$50</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="111">
   <si>
     <t>esp_code_alternatif</t>
   </si>
@@ -346,6 +346,21 @@
   </si>
   <si>
     <t>Grande alose</t>
+  </si>
+  <si>
+    <t>CR</t>
+  </si>
+  <si>
+    <t>NT</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>DD</t>
+  </si>
+  <si>
+    <t>statut_espece_lrr_2015</t>
   </si>
 </sst>
 </file>
@@ -731,10 +746,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68C65F63-35D5-4CD1-B443-72BB0835CA8F}">
-  <dimension ref="A1:E50"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:F50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -744,10 +760,11 @@
     <col min="3" max="3" width="12.5703125" style="1" customWidth="1"/>
     <col min="4" max="4" width="12.28515625" style="1" customWidth="1"/>
     <col min="5" max="5" width="19.42578125" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="11.42578125" style="1"/>
+    <col min="6" max="6" width="23.85546875" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>98</v>
       </c>
@@ -763,8 +780,11 @@
       <c r="E1" s="7" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -778,7 +798,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>0</v>
       </c>
@@ -795,7 +815,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>0</v>
       </c>
@@ -809,7 +829,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>0</v>
       </c>
@@ -823,7 +843,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>0</v>
       </c>
@@ -837,7 +857,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>0</v>
       </c>
@@ -851,7 +871,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>0</v>
       </c>
@@ -865,7 +885,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>0</v>
       </c>
@@ -879,7 +899,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>0</v>
       </c>
@@ -893,7 +913,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>0</v>
       </c>
@@ -907,7 +927,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>0</v>
       </c>
@@ -921,7 +941,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>0</v>
       </c>
@@ -935,7 +955,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>0</v>
       </c>
@@ -949,7 +969,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>0</v>
       </c>
@@ -963,7 +983,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>0</v>
       </c>
@@ -977,7 +997,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>0</v>
       </c>
@@ -991,7 +1011,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>0</v>
       </c>
@@ -1005,7 +1025,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>0</v>
       </c>
@@ -1019,7 +1039,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>0</v>
       </c>
@@ -1033,7 +1053,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>0</v>
       </c>
@@ -1047,7 +1067,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>0</v>
       </c>
@@ -1061,7 +1081,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>1</v>
       </c>
@@ -1078,7 +1098,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>1</v>
       </c>
@@ -1095,7 +1115,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>1</v>
       </c>
@@ -1112,7 +1132,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>1</v>
       </c>
@@ -1126,7 +1146,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>1</v>
       </c>
@@ -1140,10 +1160,13 @@
         <v>104</v>
       </c>
       <c r="E27" s="1">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>1</v>
       </c>
@@ -1160,7 +1183,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>1</v>
       </c>
@@ -1177,7 +1200,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>1</v>
       </c>
@@ -1193,8 +1216,11 @@
       <c r="E30" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F30" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>1</v>
       </c>
@@ -1211,7 +1237,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>1</v>
       </c>
@@ -1227,8 +1253,11 @@
       <c r="E32" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F32" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>1</v>
       </c>
@@ -1244,8 +1273,11 @@
       <c r="E33" s="1">
         <v>6</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F33" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>1</v>
       </c>
@@ -1262,7 +1294,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>1</v>
       </c>
@@ -1279,7 +1311,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>1</v>
       </c>
@@ -1293,7 +1325,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>1</v>
       </c>
@@ -1309,8 +1341,11 @@
       <c r="E37" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F37" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>1</v>
       </c>
@@ -1326,8 +1361,11 @@
       <c r="E38" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F38" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>1</v>
       </c>
@@ -1343,8 +1381,11 @@
       <c r="E39" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F39" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>1</v>
       </c>
@@ -1358,7 +1399,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>1</v>
       </c>
@@ -1374,8 +1415,11 @@
       <c r="E41" s="1">
         <v>6</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F41" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>1</v>
       </c>
@@ -1389,7 +1433,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>1</v>
       </c>
@@ -1403,7 +1447,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>1</v>
       </c>
@@ -1419,8 +1463,11 @@
       <c r="E44" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F44" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>1</v>
       </c>
@@ -1437,7 +1484,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>1</v>
       </c>
@@ -1453,8 +1500,11 @@
       <c r="E46" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F46" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>1</v>
       </c>
@@ -1471,7 +1521,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>1</v>
       </c>
@@ -1487,8 +1537,11 @@
       <c r="E48" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F48" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>1</v>
       </c>
@@ -1504,8 +1557,11 @@
       <c r="E49" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F49" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>1</v>
       </c>
@@ -1521,8 +1577,18 @@
       <c r="E50" s="1">
         <v>4</v>
       </c>
+      <c r="F50" s="1" t="s">
+        <v>109</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:F50" xr:uid="{909599AC-7C19-4796-94BF-7494204D17F1}">
+    <filterColumn colId="3">
+      <filters>
+        <filter val="indigene"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState ref="A2:C50">
     <sortCondition ref="B5"/>
   </sortState>

</xml_diff>